<commit_message>
Separated incubator 1 and 2 more clearly, cells to specific time put in incubator and temps.
</commit_message>
<xml_diff>
--- a/data/FK_MetabolismDataSheets.xlsx
+++ b/data/FK_MetabolismDataSheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="860" windowWidth="25780" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Sheet: Data</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature: </t>
   </si>
   <si>
     <t xml:space="preserve">Time placed in incubator:
@@ -172,130 +166,25 @@
     <t>Researcher:</t>
   </si>
   <si>
-    <t>ld0051</t>
-  </si>
-  <si>
-    <t>tc0140</t>
-  </si>
-  <si>
-    <t>ld0042</t>
-  </si>
-  <si>
-    <t>tc0103</t>
-  </si>
-  <si>
-    <t>ld0170</t>
-  </si>
-  <si>
-    <t>tc0415</t>
-  </si>
-  <si>
-    <t>ld0141</t>
-  </si>
-  <si>
-    <t>tc0322</t>
-  </si>
-  <si>
-    <t>ld0146</t>
-  </si>
-  <si>
-    <t>tc0340</t>
-  </si>
-  <si>
-    <t>ld0020</t>
-  </si>
-  <si>
-    <t>tc0032</t>
-  </si>
-  <si>
-    <t>ld0154</t>
-  </si>
-  <si>
-    <t>tc02(A)0</t>
-  </si>
-  <si>
-    <t>ld0118</t>
-  </si>
-  <si>
-    <t>tc0251</t>
-  </si>
-  <si>
-    <t>ld0150</t>
-  </si>
-  <si>
-    <t>tc0344</t>
-  </si>
-  <si>
-    <t>ld0140</t>
-  </si>
-  <si>
-    <t>tc0325</t>
-  </si>
-  <si>
-    <t>ld0011</t>
-  </si>
-  <si>
-    <t>tc0015</t>
-  </si>
-  <si>
-    <t>ld0018</t>
-  </si>
-  <si>
-    <t>tc0030</t>
-  </si>
-  <si>
-    <t>ld0105</t>
-  </si>
-  <si>
-    <t>tc0230</t>
-  </si>
-  <si>
-    <t>ld0002</t>
-  </si>
-  <si>
-    <t>tc0002</t>
-  </si>
-  <si>
-    <t>ld0095</t>
-  </si>
-  <si>
-    <t>tc0214</t>
-  </si>
-  <si>
-    <t>ld0088</t>
-  </si>
-  <si>
-    <t>tc0203</t>
-  </si>
-  <si>
-    <t>ld0142</t>
-  </si>
-  <si>
-    <t>tc0331</t>
-  </si>
-  <si>
-    <t>ld0049</t>
-  </si>
-  <si>
-    <t>tc01(12)0</t>
-  </si>
-  <si>
-    <t>ld0027</t>
-  </si>
-  <si>
-    <t>tc0043</t>
-  </si>
-  <si>
-    <t>ld0155</t>
-  </si>
-  <si>
-    <t>tc1342</t>
-  </si>
-  <si>
-    <t>ld0089</t>
-  </si>
-  <si>
-    <t>tc0204</t>
+    <t xml:space="preserve">Temperature 1: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature 2: </t>
+  </si>
+  <si>
+    <t>Incubator 1</t>
+  </si>
+  <si>
+    <t>Incubator 2</t>
+  </si>
+  <si>
+    <t>Air collection notes</t>
+  </si>
+  <si>
+    <t>FMS notes</t>
+  </si>
+  <si>
+    <t>Put back notes</t>
   </si>
 </sst>
 </file>
@@ -372,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -541,8 +430,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -566,14 +557,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -585,12 +583,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -608,23 +600,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -636,6 +681,11 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -647,6 +697,11 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -914,7 +969,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -925,589 +980,599 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection sqref="A1:L26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="32" customWidth="1"/>
+    <col min="12" max="14" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:14" s="17" customFormat="1">
+      <c r="A1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="G1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-    </row>
-    <row r="3" spans="1:12" ht="33" customHeight="1">
+      <c r="H1" s="28"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" ht="24" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="21"/>
-    </row>
-    <row r="4" spans="1:12" ht="32" customHeight="1">
-      <c r="A4" s="2"/>
+      <c r="G3" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="26"/>
+      <c r="K3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="1:14" ht="26" customHeight="1" thickBot="1">
+      <c r="A4" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="21"/>
-    </row>
-    <row r="5" spans="1:12" ht="16" thickBot="1">
-      <c r="A5" s="3" t="s">
+      <c r="G4" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="18"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="25" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="15">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="41"/>
+    </row>
+    <row r="7" spans="1:14" ht="25" customHeight="1">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>2</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>53</v>
-      </c>
+      <c r="K7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="41"/>
+    </row>
+    <row r="8" spans="1:14" ht="25" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>3</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="K8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="41"/>
+    </row>
+    <row r="9" spans="1:14" ht="25" customHeight="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>4</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="K9" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="41"/>
+    </row>
+    <row r="10" spans="1:14" ht="25" customHeight="1">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>5</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="K10" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="41"/>
+    </row>
+    <row r="11" spans="1:14" ht="25" customHeight="1">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>6</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="41"/>
+    </row>
+    <row r="12" spans="1:14" ht="25" customHeight="1">
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>7</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="K12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="41"/>
+    </row>
+    <row r="13" spans="1:14" ht="25" customHeight="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>8</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>65</v>
-      </c>
+      <c r="K13" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="41"/>
+    </row>
+    <row r="14" spans="1:14" ht="25" customHeight="1">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>9</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" ht="16" thickBot="1">
-      <c r="A15" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="16">
+      <c r="K14" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="41"/>
+    </row>
+    <row r="15" spans="1:14" ht="25" customHeight="1" thickBot="1">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="13">
         <v>10</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="16" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="42"/>
+    </row>
+    <row r="16" spans="1:14" ht="24" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+    </row>
+    <row r="17" spans="1:14" ht="26" customHeight="1" thickBot="1">
+      <c r="A17" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" spans="1:14" ht="25" customHeight="1">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="12">
+        <v>11</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="10"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="15">
-        <v>11</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="11">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="11">
-        <v>13</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" ht="25" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="11">
-        <v>14</v>
+      <c r="F19" s="10">
+        <v>12</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>77</v>
-      </c>
+      <c r="K19" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:14" ht="25" customHeight="1">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="11">
-        <v>15</v>
+      <c r="F20" s="10">
+        <v>13</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>79</v>
-      </c>
+      <c r="K20" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" ht="25" customHeight="1">
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="11">
-        <v>16</v>
+      <c r="F21" s="10">
+        <v>14</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>81</v>
-      </c>
+      <c r="K21" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" ht="25" customHeight="1">
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="11">
-        <v>17</v>
+      <c r="F22" s="10">
+        <v>15</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="K22" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="1:14" ht="25" customHeight="1">
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="11">
-        <v>18</v>
+      <c r="F23" s="10">
+        <v>16</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="K23" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:14" ht="25" customHeight="1">
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="11">
-        <v>19</v>
+      <c r="F24" s="10">
+        <v>17</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>87</v>
-      </c>
+      <c r="K24" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" ht="25" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="11">
-        <v>20</v>
+      <c r="F25" s="10">
+        <v>18</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" ht="25" customHeight="1">
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="10">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" ht="25" customHeight="1">
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="10">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="7"/>
+    </row>
+    <row r="28" spans="1:14" ht="25" customHeight="1" thickBot="1">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="13">
+        <v>21</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" ht="16" thickBot="1">
-      <c r="A26" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="16">
-        <v>21</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="L26" s="10"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="G3:H3"/>
@@ -1519,7 +1584,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
@@ -1542,57 +1607,57 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the width and formatting
</commit_message>
<xml_diff>
--- a/data/FK_MetabolismDataSheets.xlsx
+++ b/data/FK_MetabolismDataSheets.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="MetaData" sheetId="2" r:id="rId2"/>
+    <sheet name="Batch 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Batch 2" sheetId="3" r:id="rId2"/>
+    <sheet name="MetaData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="140">
   <si>
     <t>ID</t>
   </si>
@@ -154,9 +155,6 @@
 </t>
   </si>
   <si>
-    <t>Batch:</t>
-  </si>
-  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -185,13 +183,278 @@
   </si>
   <si>
     <t>Put back notes</t>
+  </si>
+  <si>
+    <t>Pee: Y / N
+Poop: Y / N</t>
+  </si>
+  <si>
+    <t>ld0140</t>
+  </si>
+  <si>
+    <t>tc0325</t>
+  </si>
+  <si>
+    <t>ld0020</t>
+  </si>
+  <si>
+    <t>tc0032</t>
+  </si>
+  <si>
+    <t>ld0146</t>
+  </si>
+  <si>
+    <t>tc0340</t>
+  </si>
+  <si>
+    <t>ld0150</t>
+  </si>
+  <si>
+    <t>tc0344</t>
+  </si>
+  <si>
+    <t>ld0051</t>
+  </si>
+  <si>
+    <t>tc0140</t>
+  </si>
+  <si>
+    <t>ld0095</t>
+  </si>
+  <si>
+    <t>tc0214</t>
+  </si>
+  <si>
+    <t>ld0011</t>
+  </si>
+  <si>
+    <t>tc0015</t>
+  </si>
+  <si>
+    <t>ld0027</t>
+  </si>
+  <si>
+    <t>tc0043</t>
+  </si>
+  <si>
+    <t>ld0042</t>
+  </si>
+  <si>
+    <t>tc0103</t>
+  </si>
+  <si>
+    <t>ld0170</t>
+  </si>
+  <si>
+    <t>tc0415</t>
+  </si>
+  <si>
+    <t>ld0002</t>
+  </si>
+  <si>
+    <t>tc0002</t>
+  </si>
+  <si>
+    <t>ld0154</t>
+  </si>
+  <si>
+    <t>tc02(A)0</t>
+  </si>
+  <si>
+    <t>ld0118</t>
+  </si>
+  <si>
+    <t>tc0251</t>
+  </si>
+  <si>
+    <t>ld0155</t>
+  </si>
+  <si>
+    <t>tc1342</t>
+  </si>
+  <si>
+    <t>ld0018</t>
+  </si>
+  <si>
+    <t>tc0A30</t>
+  </si>
+  <si>
+    <t>ld0049</t>
+  </si>
+  <si>
+    <t>tc01(12)0</t>
+  </si>
+  <si>
+    <t>ld0105</t>
+  </si>
+  <si>
+    <t>tc0230</t>
+  </si>
+  <si>
+    <t>ld0133</t>
+  </si>
+  <si>
+    <t>tc0314</t>
+  </si>
+  <si>
+    <t>ld0142</t>
+  </si>
+  <si>
+    <t>tc0331</t>
+  </si>
+  <si>
+    <t>ld0089</t>
+  </si>
+  <si>
+    <t>tc0204</t>
+  </si>
+  <si>
+    <t>ld0088</t>
+  </si>
+  <si>
+    <t>tc0203</t>
+  </si>
+  <si>
+    <t>Batch: 1</t>
+  </si>
+  <si>
+    <t>ld0153</t>
+  </si>
+  <si>
+    <t>tc0350</t>
+  </si>
+  <si>
+    <t>ld0128</t>
+  </si>
+  <si>
+    <t>tc0305</t>
+  </si>
+  <si>
+    <t>ld0006</t>
+  </si>
+  <si>
+    <t>tc0010</t>
+  </si>
+  <si>
+    <t>ld0092</t>
+  </si>
+  <si>
+    <t>tc0212</t>
+  </si>
+  <si>
+    <t>ld0111</t>
+  </si>
+  <si>
+    <t>tc0242</t>
+  </si>
+  <si>
+    <t>ld0076</t>
+  </si>
+  <si>
+    <t>tc0150</t>
+  </si>
+  <si>
+    <t>ld0171</t>
+  </si>
+  <si>
+    <t>tc0311</t>
+  </si>
+  <si>
+    <t>ld0138</t>
+  </si>
+  <si>
+    <t>tc0323</t>
+  </si>
+  <si>
+    <t>ld0069</t>
+  </si>
+  <si>
+    <t>tc0142</t>
+  </si>
+  <si>
+    <t>ld0043</t>
+  </si>
+  <si>
+    <t>tc0104</t>
+  </si>
+  <si>
+    <t>Batch: 2</t>
+  </si>
+  <si>
+    <t>ld0107</t>
+  </si>
+  <si>
+    <t>tc0232</t>
+  </si>
+  <si>
+    <t>ld0175</t>
+  </si>
+  <si>
+    <t>tc0234</t>
+  </si>
+  <si>
+    <t>ld0137</t>
+  </si>
+  <si>
+    <t>tc0322</t>
+  </si>
+  <si>
+    <t>ld0075</t>
+  </si>
+  <si>
+    <t>tc0145</t>
+  </si>
+  <si>
+    <t>ld0013</t>
+  </si>
+  <si>
+    <t>tc0021</t>
+  </si>
+  <si>
+    <t>ld0065</t>
+  </si>
+  <si>
+    <t>tc0134</t>
+  </si>
+  <si>
+    <t>ld0104</t>
+  </si>
+  <si>
+    <t>tc0225</t>
+  </si>
+  <si>
+    <t>ld0077</t>
+  </si>
+  <si>
+    <t>tc0151</t>
+  </si>
+  <si>
+    <t>ld0119</t>
+  </si>
+  <si>
+    <t>tc0252</t>
+  </si>
+  <si>
+    <t>ld0115</t>
+  </si>
+  <si>
+    <t>tc0244</t>
+  </si>
+  <si>
+    <t>ld0143</t>
+  </si>
+  <si>
+    <t>tc0333</t>
+  </si>
+  <si>
+    <t>Period: 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,6 +515,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -261,7 +531,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -499,7 +769,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
@@ -508,32 +780,17 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -567,8 +824,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -579,17 +854,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -621,6 +887,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -630,46 +923,62 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -686,6 +995,15 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -702,6 +1020,15 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -969,7 +1296,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -982,609 +1309,740 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="12" max="14" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="37" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="17" customFormat="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:14" s="14" customFormat="1">
+      <c r="A1" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="34"/>
+      <c r="G1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="M2" s="36"/>
     </row>
     <row r="3" spans="1:14" ht="24" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26" t="s">
+      <c r="H3" s="32"/>
+      <c r="I3" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="11" t="s">
+      <c r="J3" s="32"/>
+      <c r="K3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="18"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:14" ht="26" customHeight="1" thickBot="1">
-      <c r="A4" s="15" t="s">
-        <v>48</v>
+      <c r="A4" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33" t="s">
+      <c r="J4" s="31"/>
+      <c r="K4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="18"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="1:14" ht="16" thickBot="1">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="40" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="25" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
+    </row>
+    <row r="6" spans="1:14" ht="40" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="12">
+      <c r="F6" s="17">
         <v>1</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="29" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="44" t="s">
         <v>18</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="41"/>
-    </row>
-    <row r="7" spans="1:14" ht="25" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
+      <c r="M6" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" ht="40" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="10">
+      <c r="F7" s="19">
         <v>2</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="30" t="s">
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="41"/>
-    </row>
-    <row r="8" spans="1:14" ht="25" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
+      <c r="M7" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" ht="40" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="10">
+      <c r="F8" s="19">
         <v>3</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="30" t="s">
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="41"/>
-    </row>
-    <row r="9" spans="1:14" ht="25" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
+      <c r="M8" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" ht="40" customHeight="1">
+      <c r="A9" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="10">
+      <c r="F9" s="19">
         <v>4</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="30" t="s">
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="46" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="41"/>
-    </row>
-    <row r="10" spans="1:14" ht="25" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
+      <c r="M9" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="40" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="10">
+      <c r="F10" s="19">
         <v>5</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="30" t="s">
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="41"/>
-    </row>
-    <row r="11" spans="1:14" ht="25" customHeight="1">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
+      <c r="M10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" ht="40" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="10">
+      <c r="F11" s="19">
         <v>6</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="30" t="s">
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="41"/>
-    </row>
-    <row r="12" spans="1:14" ht="25" customHeight="1">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
+      <c r="M11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" ht="40" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="10">
+      <c r="F12" s="19">
         <v>7</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="30" t="s">
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="41"/>
-    </row>
-    <row r="13" spans="1:14" ht="25" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
+      <c r="M12" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" ht="40" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>68</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="10">
+      <c r="F13" s="19">
         <v>8</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="30" t="s">
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="46" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="41"/>
-    </row>
-    <row r="14" spans="1:14" ht="25" customHeight="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
+      <c r="M13" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" ht="40" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="10">
+      <c r="F14" s="19">
         <v>9</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="30" t="s">
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46" t="s">
         <v>27</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="41"/>
-    </row>
-    <row r="15" spans="1:14" ht="25" customHeight="1" thickBot="1">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
+      <c r="M14" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" ht="40" customHeight="1" thickBot="1">
+      <c r="A15" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="13">
+      <c r="F15" s="21">
         <v>10</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="31" t="s">
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="48" t="s">
         <v>25</v>
       </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="42"/>
+      <c r="M15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="9"/>
     </row>
     <row r="16" spans="1:14" ht="24" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="34" t="s">
+      <c r="G16" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="15"/>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" spans="1:14" ht="26" customHeight="1" thickBot="1">
-      <c r="A17" s="25" t="s">
-        <v>49</v>
+      <c r="A17" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" s="32"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-    </row>
-    <row r="18" spans="1:14" ht="25" customHeight="1">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="15"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" ht="40" customHeight="1">
+      <c r="A18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>74</v>
+      </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="12">
+      <c r="F18" s="17">
         <v>11</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="29" t="s">
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="44" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="M18" s="40" t="s">
+        <v>52</v>
+      </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="25" customHeight="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
+    <row r="19" spans="1:14" ht="40" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>76</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="10">
+      <c r="F19" s="19">
         <v>12</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="30" t="s">
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46" t="s">
         <v>28</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="M19" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" ht="25" customHeight="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
+    <row r="20" spans="1:14" ht="40" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="10">
+      <c r="F20" s="19">
         <v>13</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="30" t="s">
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="46" t="s">
         <v>29</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="M20" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="25" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
+    <row r="21" spans="1:14" ht="40" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="10">
+      <c r="F21" s="19">
         <v>14</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="30" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="M21" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" ht="25" customHeight="1">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
+    <row r="22" spans="1:14" ht="40" customHeight="1">
+      <c r="A22" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="10">
+      <c r="F22" s="19">
         <v>15</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="30" t="s">
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="46" t="s">
         <v>31</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="M22" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="25" customHeight="1">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
+    <row r="23" spans="1:14" ht="40" customHeight="1">
+      <c r="A23" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="10">
+      <c r="F23" s="19">
         <v>16</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="30" t="s">
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46" t="s">
         <v>32</v>
       </c>
       <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="M23" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" ht="25" customHeight="1">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
+    <row r="24" spans="1:14" ht="40" customHeight="1">
+      <c r="A24" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="10">
+      <c r="F24" s="19">
         <v>17</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="30" t="s">
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="46" t="s">
         <v>33</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="M24" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" ht="25" customHeight="1">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
+    <row r="25" spans="1:14" ht="40" customHeight="1">
+      <c r="A25" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>88</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="10">
+      <c r="F25" s="19">
         <v>18</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="30" t="s">
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="46" t="s">
         <v>34</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="M25" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" ht="25" customHeight="1">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+    <row r="26" spans="1:14" ht="40" customHeight="1">
+      <c r="A26" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>90</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="10">
+      <c r="F26" s="19">
         <v>19</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="30" t="s">
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="46" t="s">
         <v>35</v>
       </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="M26" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" ht="25" customHeight="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="22"/>
+    <row r="27" spans="1:14" ht="40" customHeight="1">
+      <c r="A27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="10">
+      <c r="F27" s="19">
         <v>20</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="30" t="s">
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="46" t="s">
         <v>36</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="M27" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" ht="25" customHeight="1" thickBot="1">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
+    <row r="28" spans="1:14" ht="40" customHeight="1" thickBot="1">
+      <c r="A28" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="13">
+      <c r="F28" s="21">
         <v>21</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="31" t="s">
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="48" t="s">
         <v>37</v>
       </c>
       <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="M28" s="41" t="s">
+        <v>52</v>
+      </c>
       <c r="N28" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="48" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
@@ -1598,6 +2056,761 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection sqref="A1:N28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14" s="14" customFormat="1">
+      <c r="A1" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="34"/>
+      <c r="G1" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="24"/>
+      <c r="I1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="35"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="28">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="32"/>
+      <c r="K3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="15"/>
+      <c r="M3" s="37"/>
+    </row>
+    <row r="4" spans="1:14" ht="43" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="31"/>
+      <c r="K4" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="15"/>
+      <c r="M4" s="37"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="A5" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30">
+      <c r="A6" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" ht="30">
+      <c r="A7" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="19">
+        <v>2</v>
+      </c>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" ht="30">
+      <c r="A8" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="19">
+        <v>3</v>
+      </c>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" ht="30">
+      <c r="A9" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="19">
+        <v>4</v>
+      </c>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="30">
+      <c r="A10" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="19">
+        <v>5</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" ht="30">
+      <c r="A11" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="19">
+        <v>6</v>
+      </c>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" ht="30">
+      <c r="A12" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="19">
+        <v>7</v>
+      </c>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" ht="30">
+      <c r="A13" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="19">
+        <v>8</v>
+      </c>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" ht="30">
+      <c r="A14" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="19">
+        <v>9</v>
+      </c>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" ht="31" thickBot="1">
+      <c r="A15" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="21">
+        <v>10</v>
+      </c>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="30"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" ht="16" thickBot="1">
+      <c r="A17" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="31"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" ht="30">
+      <c r="A18" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="17">
+        <v>11</v>
+      </c>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" ht="30">
+      <c r="A19" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="19">
+        <v>12</v>
+      </c>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:14" ht="30">
+      <c r="A20" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="19">
+        <v>13</v>
+      </c>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" ht="30">
+      <c r="A21" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="19">
+        <v>14</v>
+      </c>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" ht="30">
+      <c r="A22" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="19">
+        <v>15</v>
+      </c>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="1:14" ht="30">
+      <c r="A23" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="19">
+        <v>16</v>
+      </c>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:14" ht="30">
+      <c r="A24" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="19">
+        <v>17</v>
+      </c>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" ht="30">
+      <c r="A25" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="19">
+        <v>18</v>
+      </c>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" ht="30">
+      <c r="A26" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="19">
+        <v>19</v>
+      </c>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" ht="30">
+      <c r="A27" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="19">
+        <v>20</v>
+      </c>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="7"/>
+    </row>
+    <row r="28" spans="1:14" ht="31" thickBot="1">
+      <c r="A28" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="21">
+        <v>21</v>
+      </c>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="8"/>
+      <c r="M28" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
set up for sampling period 5
</commit_message>
<xml_diff>
--- a/data/FK_MetabolismDataSheets.xlsx
+++ b/data/FK_MetabolismDataSheets.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Batch 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Batch one" sheetId="3" r:id="rId1"/>
+    <sheet name="Batch two" sheetId="1" r:id="rId2"/>
     <sheet name="MetaData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -447,14 +447,14 @@
     <t>tc0333</t>
   </si>
   <si>
-    <t>Period: 3</t>
+    <t>Period: 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -515,13 +515,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -531,7 +524,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -778,19 +771,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -842,8 +824,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -887,26 +877,74 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -914,71 +952,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1004,6 +988,10 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1029,6 +1017,10 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1296,7 +1288,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1309,72 +1301,82 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="I20" workbookViewId="0">
+      <selection activeCell="N28" sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="37" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" customWidth="1"/>
+    <col min="3" max="5" width="14.1640625" customWidth="1"/>
+    <col min="7" max="10" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="37.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="40" customHeight="1">
+      <c r="A1" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="33" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="23" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="24"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-      <c r="M1" s="35"/>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
+      <c r="M1" s="30"/>
+    </row>
+    <row r="2" spans="1:14" ht="40" customHeight="1">
+      <c r="A2" s="2"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-      <c r="M2" s="36"/>
-    </row>
-    <row r="3" spans="1:14" ht="24" customHeight="1">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="40" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32" t="s">
+      <c r="H3" s="50"/>
+      <c r="I3" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="32"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="10" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="15"/>
-    </row>
-    <row r="4" spans="1:14" ht="26" customHeight="1" thickBot="1">
+      <c r="M3" s="32"/>
+    </row>
+    <row r="4" spans="1:14" ht="40" customHeight="1" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>47</v>
       </c>
@@ -1383,69 +1385,70 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31" t="s">
+      <c r="H4" s="47"/>
+      <c r="I4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="31"/>
-      <c r="K4" s="25" t="s">
+      <c r="J4" s="47"/>
+      <c r="K4" s="23" t="s">
         <v>41</v>
       </c>
       <c r="L4" s="15"/>
+      <c r="M4" s="32"/>
     </row>
     <row r="5" spans="1:14" ht="16" thickBot="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="42" t="s">
+      <c r="N5" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="40" customHeight="1">
+    <row r="6" spans="1:14" ht="30">
       <c r="A6" s="18" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1453,25 +1456,25 @@
       <c r="F6" s="17">
         <v>1</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="39" t="s">
         <v>18</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="40" customHeight="1">
+    <row r="7" spans="1:14" ht="30">
       <c r="A7" s="18" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1479,20 +1482,20 @@
       <c r="F7" s="19">
         <v>2</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46" t="s">
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="41" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:14" ht="40" customHeight="1">
+    <row r="8" spans="1:14" ht="30">
       <c r="A8" s="18" t="s">
         <v>57</v>
       </c>
@@ -1505,25 +1508,25 @@
       <c r="F8" s="19">
         <v>3</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46" t="s">
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:14" ht="40" customHeight="1">
+    <row r="9" spans="1:14" ht="30">
       <c r="A9" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1531,25 +1534,25 @@
       <c r="F9" s="19">
         <v>4</v>
       </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="46" t="s">
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:14" ht="40" customHeight="1">
+    <row r="10" spans="1:14" ht="30">
       <c r="A10" s="18" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1557,20 +1560,20 @@
       <c r="F10" s="19">
         <v>5</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="46" t="s">
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="41" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="40" customHeight="1">
+    <row r="11" spans="1:14" ht="30">
       <c r="A11" s="18" t="s">
         <v>63</v>
       </c>
@@ -1583,25 +1586,25 @@
       <c r="F11" s="19">
         <v>6</v>
       </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="46" t="s">
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="41" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:14" ht="40" customHeight="1">
+    <row r="12" spans="1:14" ht="30">
       <c r="A12" s="18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1609,25 +1612,25 @@
       <c r="F12" s="19">
         <v>7</v>
       </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="46" t="s">
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="41" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="39" t="s">
+      <c r="M12" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:14" ht="40" customHeight="1">
+    <row r="13" spans="1:14" ht="30">
       <c r="A13" s="18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1635,25 +1638,25 @@
       <c r="F13" s="19">
         <v>8</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="46" t="s">
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:14" ht="40" customHeight="1">
+    <row r="14" spans="1:14" ht="30">
       <c r="A14" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1661,25 +1664,25 @@
       <c r="F14" s="19">
         <v>9</v>
       </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46" t="s">
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="41" t="s">
         <v>27</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="39" t="s">
+      <c r="M14" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:14" ht="40" customHeight="1" thickBot="1">
+    <row r="15" spans="1:14" ht="31" thickBot="1">
       <c r="A15" s="20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1687,39 +1690,40 @@
       <c r="F15" s="21">
         <v>10</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="48" t="s">
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43" t="s">
         <v>25</v>
       </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="36" t="s">
         <v>52</v>
       </c>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:14" ht="24" customHeight="1">
+    <row r="16" spans="1:14" ht="40" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30" t="s">
+      <c r="H16" s="46"/>
+      <c r="I16" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="26"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="24"/>
       <c r="L16" s="15"/>
+      <c r="M16" s="32"/>
       <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="1:14" ht="26" customHeight="1" thickBot="1">
+    <row r="17" spans="1:14" ht="40" customHeight="1" thickBot="1">
       <c r="A17" s="22" t="s">
         <v>48</v>
       </c>
@@ -1728,24 +1732,25 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31" t="s">
+      <c r="H17" s="47"/>
+      <c r="I17" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="25"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="15"/>
+      <c r="M17" s="32"/>
       <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="1:14" ht="40" customHeight="1">
+    <row r="18" spans="1:14" ht="30">
       <c r="A18" s="16" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1753,25 +1758,25 @@
       <c r="F18" s="17">
         <v>11</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="44" t="s">
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="5"/>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="35" t="s">
         <v>52</v>
       </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="40" customHeight="1">
+    <row r="19" spans="1:14" ht="30">
       <c r="A19" s="18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1779,25 +1784,25 @@
       <c r="F19" s="19">
         <v>12</v>
       </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="46" t="s">
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="41" t="s">
         <v>28</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="39" t="s">
+      <c r="M19" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" ht="40" customHeight="1">
+    <row r="20" spans="1:14" ht="30">
       <c r="A20" s="18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1805,25 +1810,25 @@
       <c r="F20" s="19">
         <v>13</v>
       </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="46" t="s">
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="41" t="s">
         <v>29</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="39" t="s">
+      <c r="M20" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="40" customHeight="1">
+    <row r="21" spans="1:14" ht="30">
       <c r="A21" s="18" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1831,25 +1836,25 @@
       <c r="F21" s="19">
         <v>14</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="46" t="s">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="41" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="39" t="s">
+      <c r="M21" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" ht="40" customHeight="1">
+    <row r="22" spans="1:14" ht="30">
       <c r="A22" s="18" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1857,25 +1862,25 @@
       <c r="F22" s="19">
         <v>15</v>
       </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="46" t="s">
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="41" t="s">
         <v>31</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="39" t="s">
+      <c r="M22" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="40" customHeight="1">
+    <row r="23" spans="1:14" ht="30">
       <c r="A23" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1883,25 +1888,25 @@
       <c r="F23" s="19">
         <v>16</v>
       </c>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="46" t="s">
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="41" t="s">
         <v>32</v>
       </c>
       <c r="L23" s="1"/>
-      <c r="M23" s="39" t="s">
+      <c r="M23" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" ht="40" customHeight="1">
+    <row r="24" spans="1:14" ht="30">
       <c r="A24" s="18" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1909,25 +1914,25 @@
       <c r="F24" s="19">
         <v>17</v>
       </c>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="46" t="s">
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="41" t="s">
         <v>33</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="39" t="s">
+      <c r="M24" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" ht="40" customHeight="1">
+    <row r="25" spans="1:14" ht="30">
       <c r="A25" s="18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1935,25 +1940,25 @@
       <c r="F25" s="19">
         <v>18</v>
       </c>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="46" t="s">
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="41" t="s">
         <v>34</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="39" t="s">
+      <c r="M25" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" ht="40" customHeight="1">
+    <row r="26" spans="1:14" ht="30">
       <c r="A26" s="18" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1961,25 +1966,25 @@
       <c r="F26" s="19">
         <v>19</v>
       </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="46" t="s">
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="41" t="s">
         <v>35</v>
       </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="39" t="s">
+      <c r="M26" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" ht="40" customHeight="1">
+    <row r="27" spans="1:14" ht="30">
       <c r="A27" s="18" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1987,25 +1992,25 @@
       <c r="F27" s="19">
         <v>20</v>
       </c>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="46" t="s">
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41" t="s">
         <v>36</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="39" t="s">
+      <c r="M27" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" ht="40" customHeight="1" thickBot="1">
+    <row r="28" spans="1:14" ht="31" thickBot="1">
       <c r="A28" s="20" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2013,26 +2018,26 @@
       <c r="F28" s="21">
         <v>21</v>
       </c>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="48" t="s">
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="43" t="s">
         <v>37</v>
       </c>
       <c r="L28" s="8"/>
-      <c r="M28" s="41" t="s">
+      <c r="M28" s="36" t="s">
         <v>52</v>
       </c>
       <c r="N28" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="G17:H17"/>
@@ -2041,11 +2046,8 @@
     <mergeCell ref="I4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="48" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="8" max="1048575" man="1"/>
-  </colBreaks>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -2061,75 +2063,73 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:N28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N28" sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="5" width="15.33203125" customWidth="1"/>
+    <col min="7" max="10" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="36" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="35" customHeight="1">
+      <c r="A1" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="33" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="23" t="s">
+      <c r="H1" s="45"/>
+      <c r="I1" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="24"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-      <c r="M1" s="35"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2"/>
+      <c r="M1" s="30"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="28">
+      <c r="M2" s="31"/>
+    </row>
+    <row r="3" spans="1:14" ht="35" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32" t="s">
+      <c r="H3" s="50"/>
+      <c r="I3" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="32"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="10" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="15"/>
-      <c r="M3" s="37"/>
-    </row>
-    <row r="4" spans="1:14" ht="43" thickBot="1">
+    </row>
+    <row r="4" spans="1:14" ht="35" customHeight="1" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>47</v>
       </c>
@@ -2138,70 +2138,69 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31" t="s">
+      <c r="H4" s="47"/>
+      <c r="I4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="31"/>
-      <c r="K4" s="25" t="s">
+      <c r="J4" s="47"/>
+      <c r="K4" s="23" t="s">
         <v>41</v>
       </c>
       <c r="L4" s="15"/>
-      <c r="M4" s="37"/>
     </row>
     <row r="5" spans="1:14" ht="16" thickBot="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="42" t="s">
+      <c r="N5" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30">
-      <c r="A6" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>97</v>
+    <row r="6" spans="1:14" ht="40" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2209,25 +2208,25 @@
       <c r="F6" s="17">
         <v>1</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="39" t="s">
         <v>18</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="30">
-      <c r="A7" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="52" t="s">
-        <v>99</v>
+    <row r="7" spans="1:14" ht="40" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2235,24 +2234,24 @@
       <c r="F7" s="19">
         <v>2</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46" t="s">
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="41" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:14" ht="30">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:14" ht="40" customHeight="1">
+      <c r="A8" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="19" t="s">
         <v>101</v>
       </c>
       <c r="C8" s="1"/>
@@ -2261,24 +2260,24 @@
       <c r="F8" s="19">
         <v>3</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46" t="s">
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:14" ht="30">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:14" ht="40" customHeight="1">
+      <c r="A9" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="19" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="1"/>
@@ -2287,24 +2286,24 @@
       <c r="F9" s="19">
         <v>4</v>
       </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="46" t="s">
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:14" ht="30">
-      <c r="A10" s="49" t="s">
+    <row r="10" spans="1:14" ht="40" customHeight="1">
+      <c r="A10" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="19" t="s">
         <v>105</v>
       </c>
       <c r="C10" s="1"/>
@@ -2313,25 +2312,25 @@
       <c r="F10" s="19">
         <v>5</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="46" t="s">
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="41" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="30">
-      <c r="A11" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>107</v>
+    <row r="11" spans="1:14" ht="40" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2339,25 +2338,25 @@
       <c r="F11" s="19">
         <v>6</v>
       </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="46" t="s">
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="41" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:14" ht="30">
-      <c r="A12" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>109</v>
+    <row r="12" spans="1:14" ht="40" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2365,25 +2364,25 @@
       <c r="F12" s="19">
         <v>7</v>
       </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="46" t="s">
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="41" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="39" t="s">
+      <c r="M12" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:14" ht="30">
-      <c r="A13" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13" s="52" t="s">
-        <v>111</v>
+    <row r="13" spans="1:14" ht="40" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2391,25 +2390,25 @@
       <c r="F13" s="19">
         <v>8</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="46" t="s">
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:14" ht="30">
-      <c r="A14" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>113</v>
+    <row r="14" spans="1:14" ht="40" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2417,25 +2416,25 @@
       <c r="F14" s="19">
         <v>9</v>
       </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46" t="s">
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="41" t="s">
         <v>27</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="39" t="s">
+      <c r="M14" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:14" ht="31" thickBot="1">
-      <c r="A15" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>115</v>
+    <row r="15" spans="1:14" ht="40" customHeight="1" thickBot="1">
+      <c r="A15" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2443,40 +2442,39 @@
       <c r="F15" s="21">
         <v>10</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="48" t="s">
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43" t="s">
         <v>25</v>
       </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="36" t="s">
         <v>52</v>
       </c>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="35" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30" t="s">
+      <c r="H16" s="46"/>
+      <c r="I16" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="26"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="24"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="37"/>
       <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1">
+    <row r="17" spans="1:14" ht="35" customHeight="1" thickBot="1">
       <c r="A17" s="22" t="s">
         <v>48</v>
       </c>
@@ -2485,25 +2483,24 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31" t="s">
+      <c r="H17" s="47"/>
+      <c r="I17" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="25"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="37"/>
       <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="1:14" ht="30">
-      <c r="A18" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>118</v>
+    <row r="18" spans="1:14" ht="40" customHeight="1">
+      <c r="A18" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>113</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2511,25 +2508,25 @@
       <c r="F18" s="17">
         <v>11</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="44" t="s">
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="5"/>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="35" t="s">
         <v>52</v>
       </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="30">
-      <c r="A19" s="19" t="s">
-        <v>119</v>
+    <row r="19" spans="1:14" ht="40" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>131</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2537,25 +2534,25 @@
       <c r="F19" s="19">
         <v>12</v>
       </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="46" t="s">
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="41" t="s">
         <v>28</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="39" t="s">
+      <c r="M19" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" ht="30">
-      <c r="A20" s="19" t="s">
-        <v>121</v>
+    <row r="20" spans="1:14" ht="40" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2563,25 +2560,25 @@
       <c r="F20" s="19">
         <v>13</v>
       </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="46" t="s">
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="41" t="s">
         <v>29</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="39" t="s">
+      <c r="M20" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="30">
-      <c r="A21" s="19" t="s">
-        <v>123</v>
+    <row r="21" spans="1:14" ht="40" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2589,25 +2586,25 @@
       <c r="F21" s="19">
         <v>14</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="46" t="s">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="41" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="39" t="s">
+      <c r="M21" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" ht="30">
-      <c r="A22" s="19" t="s">
-        <v>125</v>
+    <row r="22" spans="1:14" ht="40" customHeight="1">
+      <c r="A22" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2615,25 +2612,25 @@
       <c r="F22" s="19">
         <v>15</v>
       </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="46" t="s">
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="41" t="s">
         <v>31</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="39" t="s">
+      <c r="M22" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="30">
-      <c r="A23" s="19" t="s">
-        <v>127</v>
+    <row r="23" spans="1:14" ht="40" customHeight="1">
+      <c r="A23" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2641,25 +2638,25 @@
       <c r="F23" s="19">
         <v>16</v>
       </c>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="46" t="s">
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="41" t="s">
         <v>32</v>
       </c>
       <c r="L23" s="1"/>
-      <c r="M23" s="39" t="s">
+      <c r="M23" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" ht="30">
-      <c r="A24" s="19" t="s">
-        <v>129</v>
+    <row r="24" spans="1:14" ht="40" customHeight="1">
+      <c r="A24" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2667,25 +2664,25 @@
       <c r="F24" s="19">
         <v>17</v>
       </c>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="46" t="s">
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="41" t="s">
         <v>33</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="39" t="s">
+      <c r="M24" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" ht="30">
-      <c r="A25" s="19" t="s">
-        <v>131</v>
+    <row r="25" spans="1:14" ht="40" customHeight="1">
+      <c r="A25" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2693,25 +2690,25 @@
       <c r="F25" s="19">
         <v>18</v>
       </c>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="46" t="s">
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="41" t="s">
         <v>34</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="39" t="s">
+      <c r="M25" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" ht="30">
-      <c r="A26" s="19" t="s">
-        <v>133</v>
+    <row r="26" spans="1:14" ht="40" customHeight="1">
+      <c r="A26" s="18" t="s">
+        <v>121</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2719,25 +2716,25 @@
       <c r="F26" s="19">
         <v>19</v>
       </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="46" t="s">
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="41" t="s">
         <v>35</v>
       </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="39" t="s">
+      <c r="M26" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" ht="30">
-      <c r="A27" s="19" t="s">
-        <v>135</v>
+    <row r="27" spans="1:14" ht="40" customHeight="1">
+      <c r="A27" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2745,24 +2742,24 @@
       <c r="F27" s="19">
         <v>20</v>
       </c>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="46" t="s">
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41" t="s">
         <v>36</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="39" t="s">
+      <c r="M27" s="34" t="s">
         <v>52</v>
       </c>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" ht="31" thickBot="1">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:14" ht="40" customHeight="1" thickBot="1">
+      <c r="A28" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="21" t="s">
         <v>138</v>
       </c>
       <c r="C28" s="8"/>
@@ -2771,15 +2768,15 @@
       <c r="F28" s="21">
         <v>21</v>
       </c>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="48" t="s">
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="43" t="s">
         <v>37</v>
       </c>
       <c r="L28" s="8"/>
-      <c r="M28" s="41" t="s">
+      <c r="M28" s="36" t="s">
         <v>52</v>
       </c>
       <c r="N28" s="9"/>
@@ -2792,15 +2789,18 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="46" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="8" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Prepped for sampling period 7
</commit_message>
<xml_diff>
--- a/data/FK_MetabolismDataSheets.xlsx
+++ b/data/FK_MetabolismDataSheets.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11060" yWindow="0" windowWidth="25360" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch one" sheetId="3" r:id="rId1"/>
-    <sheet name="Batch two" sheetId="1" r:id="rId2"/>
+    <sheet name="Batch 2" sheetId="3" r:id="rId1"/>
+    <sheet name="Batch 1" sheetId="1" r:id="rId2"/>
     <sheet name="MetaData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -447,7 +447,7 @@
     <t>tc0333</t>
   </si>
   <si>
-    <t>Period: 5</t>
+    <t>Period: 7</t>
   </si>
 </sst>
 </file>
@@ -1301,8 +1301,8 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="I20" workbookViewId="0">
-      <selection activeCell="N28" sqref="A1:N28"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="D1" s="49"/>
       <c r="E1" s="48" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="28" t="s">
@@ -1445,10 +1445,10 @@
     </row>
     <row r="6" spans="1:14" ht="30">
       <c r="A6" s="18" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="7" spans="1:14" ht="30">
       <c r="A7" s="18" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1497,10 +1497,10 @@
     </row>
     <row r="8" spans="1:14" ht="30">
       <c r="A8" s="18" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1523,10 +1523,10 @@
     </row>
     <row r="9" spans="1:14" ht="30">
       <c r="A9" s="18" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="10" spans="1:14" ht="30">
       <c r="A10" s="18" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="11" spans="1:14" ht="30">
       <c r="A11" s="18" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1601,10 +1601,10 @@
     </row>
     <row r="12" spans="1:14" ht="30">
       <c r="A12" s="18" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1627,10 +1627,10 @@
     </row>
     <row r="13" spans="1:14" ht="30">
       <c r="A13" s="18" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1653,10 +1653,10 @@
     </row>
     <row r="14" spans="1:14" ht="30">
       <c r="A14" s="18" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1679,10 +1679,10 @@
     </row>
     <row r="15" spans="1:14" ht="31" thickBot="1">
       <c r="A15" s="20" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1747,10 +1747,10 @@
     </row>
     <row r="18" spans="1:14" ht="30">
       <c r="A18" s="16" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1773,10 +1773,10 @@
     </row>
     <row r="19" spans="1:14" ht="30">
       <c r="A19" s="18" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="20" spans="1:14" ht="30">
       <c r="A20" s="18" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="21" spans="1:14" ht="30">
       <c r="A21" s="18" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1851,10 +1851,10 @@
     </row>
     <row r="22" spans="1:14" ht="30">
       <c r="A22" s="18" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1877,10 +1877,10 @@
     </row>
     <row r="23" spans="1:14" ht="30">
       <c r="A23" s="18" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1903,10 +1903,10 @@
     </row>
     <row r="24" spans="1:14" ht="30">
       <c r="A24" s="18" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="25" spans="1:14" ht="30">
       <c r="A25" s="18" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="26" spans="1:14" ht="30">
       <c r="A26" s="18" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1981,10 +1981,10 @@
     </row>
     <row r="27" spans="1:14" ht="30">
       <c r="A27" s="18" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="28" spans="1:14" ht="31" thickBot="1">
       <c r="A28" s="20" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2063,8 +2063,8 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="N28" sqref="A1:N28"/>
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="D1" s="49"/>
       <c r="E1" s="48" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="44" t="s">
@@ -2197,10 +2197,10 @@
     </row>
     <row r="6" spans="1:14" ht="40" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2223,10 +2223,10 @@
     </row>
     <row r="7" spans="1:14" ht="40" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2249,10 +2249,10 @@
     </row>
     <row r="8" spans="1:14" ht="40" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2275,10 +2275,10 @@
     </row>
     <row r="9" spans="1:14" ht="40" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2301,10 +2301,10 @@
     </row>
     <row r="10" spans="1:14" ht="40" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2327,10 +2327,10 @@
     </row>
     <row r="11" spans="1:14" ht="40" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2353,10 +2353,10 @@
     </row>
     <row r="12" spans="1:14" ht="40" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>136</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2379,10 +2379,10 @@
     </row>
     <row r="13" spans="1:14" ht="40" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2405,10 +2405,10 @@
     </row>
     <row r="14" spans="1:14" ht="40" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2431,10 +2431,10 @@
     </row>
     <row r="15" spans="1:14" ht="40" customHeight="1" thickBot="1">
       <c r="A15" s="20" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2497,10 +2497,10 @@
     </row>
     <row r="18" spans="1:14" ht="40" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2523,10 +2523,10 @@
     </row>
     <row r="19" spans="1:14" ht="40" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2549,10 +2549,10 @@
     </row>
     <row r="20" spans="1:14" ht="40" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2575,10 +2575,10 @@
     </row>
     <row r="21" spans="1:14" ht="40" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2601,10 +2601,10 @@
     </row>
     <row r="22" spans="1:14" ht="40" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2627,10 +2627,10 @@
     </row>
     <row r="23" spans="1:14" ht="40" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2653,10 +2653,10 @@
     </row>
     <row r="24" spans="1:14" ht="40" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2679,10 +2679,10 @@
     </row>
     <row r="25" spans="1:14" ht="40" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2705,10 +2705,10 @@
     </row>
     <row r="26" spans="1:14" ht="40" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2731,10 +2731,10 @@
     </row>
     <row r="27" spans="1:14" ht="40" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>129</v>
+        <v>61</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2757,10 +2757,10 @@
     </row>
     <row r="28" spans="1:14" ht="40" customHeight="1" thickBot="1">
       <c r="A28" s="20" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>

</xml_diff>

<commit_message>
Prepped for sampling period 8
</commit_message>
<xml_diff>
--- a/data/FK_MetabolismDataSheets.xlsx
+++ b/data/FK_MetabolismDataSheets.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="0" windowWidth="25360" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="5720" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch 2" sheetId="3" r:id="rId1"/>
-    <sheet name="Batch 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Batch 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Batch 2" sheetId="3" r:id="rId2"/>
     <sheet name="MetaData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -447,7 +447,7 @@
     <t>tc0333</t>
   </si>
   <si>
-    <t>Period: 7</t>
+    <t>Period: 8</t>
   </si>
 </sst>
 </file>
@@ -946,20 +946,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1288,7 +1288,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1301,7 +1301,760 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="E17" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection sqref="A1:N28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="5" width="15.33203125" customWidth="1"/>
+    <col min="7" max="10" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="36" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="35" customHeight="1">
+      <c r="A1" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="47"/>
+      <c r="E1" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="47"/>
+      <c r="G1" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="45"/>
+      <c r="I1" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="45"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="30"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="M2" s="31"/>
+    </row>
+    <row r="3" spans="1:14" ht="35" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="48"/>
+      <c r="K3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" ht="35" customHeight="1" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="50"/>
+      <c r="K4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="A5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="40" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" ht="40" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="19">
+        <v>2</v>
+      </c>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" ht="40" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="19">
+        <v>3</v>
+      </c>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" ht="40" customHeight="1">
+      <c r="A9" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="19">
+        <v>4</v>
+      </c>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="40" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="19">
+        <v>5</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" ht="40" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="19">
+        <v>6</v>
+      </c>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" ht="40" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="19">
+        <v>7</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" ht="40" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="19">
+        <v>8</v>
+      </c>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" ht="40" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="19">
+        <v>9</v>
+      </c>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" ht="40" customHeight="1" thickBot="1">
+      <c r="A15" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="21">
+        <v>10</v>
+      </c>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" ht="35" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="49"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="15"/>
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" ht="35" customHeight="1" thickBot="1">
+      <c r="A17" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="50"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="15"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" ht="40" customHeight="1">
+      <c r="A18" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="17">
+        <v>11</v>
+      </c>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" ht="40" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="19">
+        <v>12</v>
+      </c>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:14" ht="40" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="19">
+        <v>13</v>
+      </c>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" ht="40" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="19">
+        <v>14</v>
+      </c>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" ht="40" customHeight="1">
+      <c r="A22" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="19">
+        <v>15</v>
+      </c>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="1:14" ht="40" customHeight="1">
+      <c r="A23" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="19">
+        <v>16</v>
+      </c>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:14" ht="40" customHeight="1">
+      <c r="A24" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="19">
+        <v>17</v>
+      </c>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" ht="40" customHeight="1">
+      <c r="A25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="19">
+        <v>18</v>
+      </c>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" ht="40" customHeight="1">
+      <c r="A26" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="19">
+        <v>19</v>
+      </c>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" ht="40" customHeight="1">
+      <c r="A27" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="19">
+        <v>20</v>
+      </c>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="7"/>
+    </row>
+    <row r="28" spans="1:14" ht="40" customHeight="1" thickBot="1">
+      <c r="A28" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="21">
+        <v>21</v>
+      </c>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="8"/>
+      <c r="M28" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="46" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="8" max="1048575" man="1"/>
+  </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
@@ -1315,18 +2068,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="14" customFormat="1" ht="40" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="48" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="48" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="49"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="28" t="s">
         <v>43</v>
       </c>
@@ -1362,14 +2115,14 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50" t="s">
+      <c r="H3" s="48"/>
+      <c r="I3" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="50"/>
+      <c r="J3" s="48"/>
       <c r="K3" s="10" t="s">
         <v>40</v>
       </c>
@@ -1385,14 +2138,14 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47" t="s">
+      <c r="H4" s="50"/>
+      <c r="I4" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="47"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="23" t="s">
         <v>41</v>
       </c>
@@ -1445,10 +2198,10 @@
     </row>
     <row r="6" spans="1:14" ht="30">
       <c r="A6" s="18" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1471,10 +2224,10 @@
     </row>
     <row r="7" spans="1:14" ht="30">
       <c r="A7" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1497,10 +2250,10 @@
     </row>
     <row r="8" spans="1:14" ht="30">
       <c r="A8" s="18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1523,10 +2276,10 @@
     </row>
     <row r="9" spans="1:14" ht="30">
       <c r="A9" s="18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1549,10 +2302,10 @@
     </row>
     <row r="10" spans="1:14" ht="30">
       <c r="A10" s="18" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1575,10 +2328,10 @@
     </row>
     <row r="11" spans="1:14" ht="30">
       <c r="A11" s="18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1601,10 +2354,10 @@
     </row>
     <row r="12" spans="1:14" ht="30">
       <c r="A12" s="18" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1627,10 +2380,10 @@
     </row>
     <row r="13" spans="1:14" ht="30">
       <c r="A13" s="18" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1653,10 +2406,10 @@
     </row>
     <row r="14" spans="1:14" ht="30">
       <c r="A14" s="18" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1710,14 +2463,14 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="46" t="s">
+      <c r="G16" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46" t="s">
+      <c r="H16" s="49"/>
+      <c r="I16" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="46"/>
+      <c r="J16" s="49"/>
       <c r="K16" s="24"/>
       <c r="L16" s="15"/>
       <c r="M16" s="32"/>
@@ -1732,14 +2485,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="47" t="s">
+      <c r="G17" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47" t="s">
+      <c r="H17" s="50"/>
+      <c r="I17" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="47"/>
+      <c r="J17" s="50"/>
       <c r="K17" s="23"/>
       <c r="L17" s="15"/>
       <c r="M17" s="32"/>
@@ -1773,10 +2526,10 @@
     </row>
     <row r="19" spans="1:14" ht="30">
       <c r="A19" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1799,10 +2552,10 @@
     </row>
     <row r="20" spans="1:14" ht="30">
       <c r="A20" s="18" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1825,10 +2578,10 @@
     </row>
     <row r="21" spans="1:14" ht="30">
       <c r="A21" s="18" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1851,10 +2604,10 @@
     </row>
     <row r="22" spans="1:14" ht="30">
       <c r="A22" s="18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1877,10 +2630,10 @@
     </row>
     <row r="23" spans="1:14" ht="30">
       <c r="A23" s="18" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1903,10 +2656,10 @@
     </row>
     <row r="24" spans="1:14" ht="30">
       <c r="A24" s="18" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1929,10 +2682,10 @@
     </row>
     <row r="25" spans="1:14" ht="30">
       <c r="A25" s="18" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1955,10 +2708,10 @@
     </row>
     <row r="26" spans="1:14" ht="30">
       <c r="A26" s="18" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1981,10 +2734,10 @@
     </row>
     <row r="27" spans="1:14" ht="30">
       <c r="A27" s="18" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2007,760 +2760,10 @@
     </row>
     <row r="28" spans="1:14" ht="31" thickBot="1">
       <c r="A28" s="20" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="21">
-        <v>21</v>
-      </c>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="N28" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:N28"/>
-  <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:N28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="3" max="5" width="15.33203125" customWidth="1"/>
-    <col min="7" max="10" width="15.33203125" customWidth="1"/>
-    <col min="12" max="12" width="36" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" ht="35" customHeight="1">
-      <c r="A1" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="30"/>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="M2" s="31"/>
-    </row>
-    <row r="3" spans="1:14" ht="35" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="15"/>
-    </row>
-    <row r="4" spans="1:14" ht="35" customHeight="1" thickBot="1">
-      <c r="A4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1">
-      <c r="A5" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="40" customHeight="1">
-      <c r="A6" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="17">
-        <v>1</v>
-      </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" ht="40" customHeight="1">
-      <c r="A7" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="19">
-        <v>2</v>
-      </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" ht="40" customHeight="1">
-      <c r="A8" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="19">
-        <v>3</v>
-      </c>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="1:14" ht="40" customHeight="1">
-      <c r="A9" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="19">
-        <v>4</v>
-      </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:14" ht="40" customHeight="1">
-      <c r="A10" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="19">
-        <v>5</v>
-      </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="7"/>
-    </row>
-    <row r="11" spans="1:14" ht="40" customHeight="1">
-      <c r="A11" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="19">
-        <v>6</v>
-      </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" ht="40" customHeight="1">
-      <c r="A12" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="19">
-        <v>7</v>
-      </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" ht="40" customHeight="1">
-      <c r="A13" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="19">
-        <v>8</v>
-      </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" ht="40" customHeight="1">
-      <c r="A14" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="19">
-        <v>9</v>
-      </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" ht="40" customHeight="1" thickBot="1">
-      <c r="A15" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="21">
-        <v>10</v>
-      </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="8"/>
-      <c r="M15" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" ht="35" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="46"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="15"/>
-      <c r="N16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" ht="35" customHeight="1" thickBot="1">
-      <c r="A17" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="47"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="15"/>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" ht="40" customHeight="1">
-      <c r="A18" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="17">
-        <v>11</v>
-      </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" ht="40" customHeight="1">
-      <c r="A19" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="19">
-        <v>12</v>
-      </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="1:14" ht="40" customHeight="1">
-      <c r="A20" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="19">
-        <v>13</v>
-      </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:14" ht="40" customHeight="1">
-      <c r="A21" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="19">
-        <v>14</v>
-      </c>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="1:14" ht="40" customHeight="1">
-      <c r="A22" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="19">
-        <v>15</v>
-      </c>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="1:14" ht="40" customHeight="1">
-      <c r="A23" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="19">
-        <v>16</v>
-      </c>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="1:14" ht="40" customHeight="1">
-      <c r="A24" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="19">
-        <v>17</v>
-      </c>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="L24" s="1"/>
-      <c r="M24" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N24" s="7"/>
-    </row>
-    <row r="25" spans="1:14" ht="40" customHeight="1">
-      <c r="A25" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="19">
-        <v>18</v>
-      </c>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N25" s="7"/>
-    </row>
-    <row r="26" spans="1:14" ht="40" customHeight="1">
-      <c r="A26" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="19">
-        <v>19</v>
-      </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N26" s="7"/>
-    </row>
-    <row r="27" spans="1:14" ht="40" customHeight="1">
-      <c r="A27" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="19">
-        <v>20</v>
-      </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="1"/>
-      <c r="M27" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="N27" s="7"/>
-    </row>
-    <row r="28" spans="1:14" ht="40" customHeight="1" thickBot="1">
-      <c r="A28" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2789,18 +2792,15 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="46" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="8" max="1048575" man="1"/>
-  </colBreaks>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
data set up complete for experiment.
</commit_message>
<xml_diff>
--- a/data/FK_MetabolismDataSheets.xlsx
+++ b/data/FK_MetabolismDataSheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="0" windowWidth="25360" windowHeight="14620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="14860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Batch 1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
     <t>tc0333</t>
   </si>
   <si>
-    <t>Period: 8</t>
+    <t>Period: 10</t>
   </si>
 </sst>
 </file>
@@ -946,14 +946,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1288,7 +1288,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1301,7 +1301,7 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="E17" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView topLeftCell="F16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
@@ -1315,18 +1315,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="14" customFormat="1" ht="35" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="46" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="46" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="47"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="44" t="s">
         <v>43</v>
       </c>
@@ -1354,14 +1354,14 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48" t="s">
+      <c r="H3" s="46"/>
+      <c r="I3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="48"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="10" t="s">
         <v>40</v>
       </c>
@@ -1435,10 +1435,10 @@
     </row>
     <row r="6" spans="1:14" ht="40" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1487,10 +1487,10 @@
     </row>
     <row r="8" spans="1:14" ht="40" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1513,10 +1513,10 @@
     </row>
     <row r="9" spans="1:14" ht="40" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="10" spans="1:14" ht="40" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1565,10 +1565,10 @@
     </row>
     <row r="11" spans="1:14" ht="40" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1591,10 +1591,10 @@
     </row>
     <row r="12" spans="1:14" ht="40" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1617,10 +1617,10 @@
     </row>
     <row r="13" spans="1:14" ht="40" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1643,10 +1643,10 @@
     </row>
     <row r="14" spans="1:14" ht="40" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1669,10 +1669,10 @@
     </row>
     <row r="15" spans="1:14" ht="40" customHeight="1" thickBot="1">
       <c r="A15" s="20" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1735,10 +1735,10 @@
     </row>
     <row r="18" spans="1:14" ht="40" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1761,10 +1761,10 @@
     </row>
     <row r="19" spans="1:14" ht="40" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1787,10 +1787,10 @@
     </row>
     <row r="20" spans="1:14" ht="40" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1813,10 +1813,10 @@
     </row>
     <row r="21" spans="1:14" ht="40" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1839,10 +1839,10 @@
     </row>
     <row r="22" spans="1:14" ht="40" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1865,10 +1865,10 @@
     </row>
     <row r="23" spans="1:14" ht="40" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1917,10 +1917,10 @@
     </row>
     <row r="25" spans="1:14" ht="40" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1943,10 +1943,10 @@
     </row>
     <row r="26" spans="1:14" ht="40" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1969,10 +1969,10 @@
     </row>
     <row r="27" spans="1:14" ht="40" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1995,10 +1995,10 @@
     </row>
     <row r="28" spans="1:14" ht="40" customHeight="1" thickBot="1">
       <c r="A28" s="20" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2021,17 +2021,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2054,7 +2054,7 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
@@ -2068,18 +2068,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="14" customFormat="1" ht="40" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="46" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="46" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="47"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="28" t="s">
         <v>43</v>
       </c>
@@ -2115,14 +2115,14 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48" t="s">
+      <c r="H3" s="46"/>
+      <c r="I3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="48"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="10" t="s">
         <v>40</v>
       </c>
@@ -2198,10 +2198,10 @@
     </row>
     <row r="6" spans="1:14" ht="30">
       <c r="A6" s="18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2224,10 +2224,10 @@
     </row>
     <row r="7" spans="1:14" ht="30">
       <c r="A7" s="18" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2250,10 +2250,10 @@
     </row>
     <row r="8" spans="1:14" ht="30">
       <c r="A8" s="18" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2276,10 +2276,10 @@
     </row>
     <row r="9" spans="1:14" ht="30">
       <c r="A9" s="18" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2302,10 +2302,10 @@
     </row>
     <row r="10" spans="1:14" ht="30">
       <c r="A10" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="11" spans="1:14" ht="30">
       <c r="A11" s="18" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2354,10 +2354,10 @@
     </row>
     <row r="12" spans="1:14" ht="30">
       <c r="A12" s="18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2406,10 +2406,10 @@
     </row>
     <row r="14" spans="1:14" ht="30">
       <c r="A14" s="18" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2432,10 +2432,10 @@
     </row>
     <row r="15" spans="1:14" ht="31" thickBot="1">
       <c r="A15" s="20" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2500,10 +2500,10 @@
     </row>
     <row r="18" spans="1:14" ht="30">
       <c r="A18" s="16" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2526,10 +2526,10 @@
     </row>
     <row r="19" spans="1:14" ht="30">
       <c r="A19" s="18" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2552,10 +2552,10 @@
     </row>
     <row r="20" spans="1:14" ht="30">
       <c r="A20" s="18" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2578,10 +2578,10 @@
     </row>
     <row r="21" spans="1:14" ht="30">
       <c r="A21" s="18" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2604,10 +2604,10 @@
     </row>
     <row r="22" spans="1:14" ht="30">
       <c r="A22" s="18" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2630,10 +2630,10 @@
     </row>
     <row r="23" spans="1:14" ht="30">
       <c r="A23" s="18" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2656,10 +2656,10 @@
     </row>
     <row r="24" spans="1:14" ht="30">
       <c r="A24" s="18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2682,10 +2682,10 @@
     </row>
     <row r="25" spans="1:14" ht="30">
       <c r="A25" s="18" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="26" spans="1:14" ht="30">
       <c r="A26" s="18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2734,10 +2734,10 @@
     </row>
     <row r="27" spans="1:14" ht="30">
       <c r="A27" s="18" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2760,10 +2760,10 @@
     </row>
     <row r="28" spans="1:14" ht="31" thickBot="1">
       <c r="A28" s="20" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2786,17 +2786,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>